<commit_message>
Mise à jour de l'application
</commit_message>
<xml_diff>
--- a/data/DonneesGPSPropres.xlsx
+++ b/data/DonneesGPSPropres.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophergallo/Desktop/Application perso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C589AD-6BCF-4440-8E64-E16E67F94A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8784B-8B89-2746-8601-E3ACA3249DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{D839DFFF-AA38-2145-9D48-3C82EEA1EE91}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="240">
   <si>
     <t>Temps joué</t>
   </si>
@@ -738,6 +738,24 @@
   </si>
   <si>
     <t>01:55:38</t>
+  </si>
+  <si>
+    <t>01:26:21</t>
+  </si>
+  <si>
+    <t>01:28:09</t>
+  </si>
+  <si>
+    <t>01:26:10</t>
+  </si>
+  <si>
+    <t>01:28:36</t>
+  </si>
+  <si>
+    <t>01:27:50</t>
+  </si>
+  <si>
+    <t>01:20:18</t>
   </si>
 </sst>
 </file>
@@ -818,9 +836,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -858,7 +876,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -964,7 +982,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1106,7 +1124,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1114,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AE8228-0F81-ED4B-A4A4-4C340123FE2A}">
-  <dimension ref="A1:V222"/>
+  <dimension ref="A1:V230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D227" sqref="D227"/>
+    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15561,6 +15579,526 @@
         <v>2</v>
       </c>
     </row>
+    <row r="223" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>23</v>
+      </c>
+      <c r="B223" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C223" t="s">
+        <v>20</v>
+      </c>
+      <c r="E223" t="s">
+        <v>25</v>
+      </c>
+      <c r="F223" t="s">
+        <v>29</v>
+      </c>
+      <c r="G223" t="s">
+        <v>234</v>
+      </c>
+      <c r="H223">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="I223">
+        <v>0</v>
+      </c>
+      <c r="J223">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K223">
+        <v>0</v>
+      </c>
+      <c r="L223">
+        <v>0</v>
+      </c>
+      <c r="M223">
+        <v>0</v>
+      </c>
+      <c r="N223">
+        <v>0</v>
+      </c>
+      <c r="O223">
+        <v>0</v>
+      </c>
+      <c r="P223">
+        <v>2.36</v>
+      </c>
+      <c r="Q223">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="R223">
+        <v>0</v>
+      </c>
+      <c r="S223">
+        <v>0</v>
+      </c>
+      <c r="T223">
+        <v>0</v>
+      </c>
+      <c r="U223">
+        <v>0</v>
+      </c>
+      <c r="V223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>23</v>
+      </c>
+      <c r="B224" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C224" t="s">
+        <v>20</v>
+      </c>
+      <c r="E224" t="s">
+        <v>43</v>
+      </c>
+      <c r="F224" t="s">
+        <v>34</v>
+      </c>
+      <c r="G224" t="s">
+        <v>235</v>
+      </c>
+      <c r="H224">
+        <v>7.15</v>
+      </c>
+      <c r="I224">
+        <v>1.66</v>
+      </c>
+      <c r="J224">
+        <v>5.47</v>
+      </c>
+      <c r="K224">
+        <v>0.77</v>
+      </c>
+      <c r="L224">
+        <v>0.9</v>
+      </c>
+      <c r="M224">
+        <v>0.01</v>
+      </c>
+      <c r="N224">
+        <v>0</v>
+      </c>
+      <c r="O224">
+        <v>1</v>
+      </c>
+      <c r="P224">
+        <v>4.8</v>
+      </c>
+      <c r="Q224">
+        <v>26.86</v>
+      </c>
+      <c r="R224">
+        <v>4.46</v>
+      </c>
+      <c r="S224">
+        <v>45</v>
+      </c>
+      <c r="T224">
+        <v>6</v>
+      </c>
+      <c r="U224">
+        <v>21</v>
+      </c>
+      <c r="V224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>23</v>
+      </c>
+      <c r="B225" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C225" t="s">
+        <v>20</v>
+      </c>
+      <c r="E225" t="s">
+        <v>35</v>
+      </c>
+      <c r="F225" t="s">
+        <v>34</v>
+      </c>
+      <c r="G225" t="s">
+        <v>236</v>
+      </c>
+      <c r="H225">
+        <v>7.73</v>
+      </c>
+      <c r="I225">
+        <v>1.6</v>
+      </c>
+      <c r="J225">
+        <v>6.12</v>
+      </c>
+      <c r="K225">
+        <v>1.27</v>
+      </c>
+      <c r="L225">
+        <v>0.33</v>
+      </c>
+      <c r="M225">
+        <v>0.01</v>
+      </c>
+      <c r="N225">
+        <v>0</v>
+      </c>
+      <c r="O225">
+        <v>1</v>
+      </c>
+      <c r="P225">
+        <v>5.33</v>
+      </c>
+      <c r="Q225">
+        <v>27.04</v>
+      </c>
+      <c r="R225">
+        <v>5.14</v>
+      </c>
+      <c r="S225">
+        <v>61</v>
+      </c>
+      <c r="T225">
+        <v>12</v>
+      </c>
+      <c r="U225">
+        <v>21</v>
+      </c>
+      <c r="V225">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>23</v>
+      </c>
+      <c r="B226" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C226" t="s">
+        <v>20</v>
+      </c>
+      <c r="E226" t="s">
+        <v>52</v>
+      </c>
+      <c r="F226" t="s">
+        <v>33</v>
+      </c>
+      <c r="G226" t="s">
+        <v>237</v>
+      </c>
+      <c r="H226">
+        <v>7.05</v>
+      </c>
+      <c r="I226">
+        <v>1.35</v>
+      </c>
+      <c r="J226">
+        <v>5.69</v>
+      </c>
+      <c r="K226">
+        <v>1</v>
+      </c>
+      <c r="L226">
+        <v>0.35</v>
+      </c>
+      <c r="M226">
+        <v>0.01</v>
+      </c>
+      <c r="N226">
+        <v>0</v>
+      </c>
+      <c r="O226">
+        <v>1</v>
+      </c>
+      <c r="P226">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="Q226">
+        <v>26.54</v>
+      </c>
+      <c r="R226">
+        <v>4.57</v>
+      </c>
+      <c r="S226">
+        <v>38</v>
+      </c>
+      <c r="T226">
+        <v>2</v>
+      </c>
+      <c r="U226">
+        <v>17</v>
+      </c>
+      <c r="V226">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>23</v>
+      </c>
+      <c r="B227" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C227" t="s">
+        <v>20</v>
+      </c>
+      <c r="E227" t="s">
+        <v>53</v>
+      </c>
+      <c r="F227" t="s">
+        <v>32</v>
+      </c>
+      <c r="G227" t="s">
+        <v>238</v>
+      </c>
+      <c r="H227">
+        <v>7.59</v>
+      </c>
+      <c r="I227">
+        <v>1.39</v>
+      </c>
+      <c r="J227">
+        <v>6.2</v>
+      </c>
+      <c r="K227">
+        <v>1.22</v>
+      </c>
+      <c r="L227">
+        <v>0.17</v>
+      </c>
+      <c r="M227">
+        <v>0</v>
+      </c>
+      <c r="N227">
+        <v>0</v>
+      </c>
+      <c r="O227">
+        <v>0</v>
+      </c>
+      <c r="P227">
+        <v>5.13</v>
+      </c>
+      <c r="Q227">
+        <v>24.1</v>
+      </c>
+      <c r="R227">
+        <v>4.26</v>
+      </c>
+      <c r="S227">
+        <v>30</v>
+      </c>
+      <c r="T227">
+        <v>3</v>
+      </c>
+      <c r="U227">
+        <v>12</v>
+      </c>
+      <c r="V227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>23</v>
+      </c>
+      <c r="B228" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C228" t="s">
+        <v>20</v>
+      </c>
+      <c r="E228" t="s">
+        <v>40</v>
+      </c>
+      <c r="F228" t="s">
+        <v>31</v>
+      </c>
+      <c r="G228" t="s">
+        <v>239</v>
+      </c>
+      <c r="H228">
+        <v>5.97</v>
+      </c>
+      <c r="I228">
+        <v>1.03</v>
+      </c>
+      <c r="J228">
+        <v>4.93</v>
+      </c>
+      <c r="K228">
+        <v>0.89</v>
+      </c>
+      <c r="L228">
+        <v>0.12</v>
+      </c>
+      <c r="M228">
+        <v>0.03</v>
+      </c>
+      <c r="N228">
+        <v>0</v>
+      </c>
+      <c r="O228">
+        <v>3</v>
+      </c>
+      <c r="P228">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="Q228">
+        <v>27.76</v>
+      </c>
+      <c r="R228">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="S228">
+        <v>24</v>
+      </c>
+      <c r="T228">
+        <v>10</v>
+      </c>
+      <c r="U228">
+        <v>23</v>
+      </c>
+      <c r="V228">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>23</v>
+      </c>
+      <c r="B229" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C229" t="s">
+        <v>20</v>
+      </c>
+      <c r="E229" t="s">
+        <v>39</v>
+      </c>
+      <c r="F229" t="s">
+        <v>29</v>
+      </c>
+      <c r="G229" t="s">
+        <v>148</v>
+      </c>
+      <c r="H229">
+        <v>7.13</v>
+      </c>
+      <c r="I229">
+        <v>1.44</v>
+      </c>
+      <c r="J229">
+        <v>5.69</v>
+      </c>
+      <c r="K229">
+        <v>1.24</v>
+      </c>
+      <c r="L229">
+        <v>0.2</v>
+      </c>
+      <c r="M229">
+        <v>0</v>
+      </c>
+      <c r="N229">
+        <v>0</v>
+      </c>
+      <c r="O229">
+        <v>0</v>
+      </c>
+      <c r="P229">
+        <v>4.88</v>
+      </c>
+      <c r="Q229">
+        <v>21.56</v>
+      </c>
+      <c r="R229">
+        <v>4.21</v>
+      </c>
+      <c r="S229">
+        <v>32</v>
+      </c>
+      <c r="T229">
+        <v>3</v>
+      </c>
+      <c r="U229">
+        <v>9</v>
+      </c>
+      <c r="V229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>23</v>
+      </c>
+      <c r="B230" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C230" t="s">
+        <v>20</v>
+      </c>
+      <c r="E230" t="s">
+        <v>164</v>
+      </c>
+      <c r="F230" t="s">
+        <v>32</v>
+      </c>
+      <c r="G230" t="s">
+        <v>235</v>
+      </c>
+      <c r="H230">
+        <v>6.85</v>
+      </c>
+      <c r="I230">
+        <v>1.44</v>
+      </c>
+      <c r="J230">
+        <v>5.4</v>
+      </c>
+      <c r="K230">
+        <v>1.28</v>
+      </c>
+      <c r="L230">
+        <v>0.17</v>
+      </c>
+      <c r="M230">
+        <v>0</v>
+      </c>
+      <c r="N230">
+        <v>0</v>
+      </c>
+      <c r="O230">
+        <v>0</v>
+      </c>
+      <c r="P230">
+        <v>4.45</v>
+      </c>
+      <c r="Q230">
+        <v>22.57</v>
+      </c>
+      <c r="R230">
+        <v>4.24</v>
+      </c>
+      <c r="S230">
+        <v>25</v>
+      </c>
+      <c r="T230">
+        <v>1</v>
+      </c>
+      <c r="U230">
+        <v>18</v>
+      </c>
+      <c r="V230">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>